<commit_message>
creating a list of ticker symbols
</commit_message>
<xml_diff>
--- a/fundamentals_condensed_df.xlsx
+++ b/fundamentals_condensed_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25ac2033dcfcea55/Desktop/ALIENWARE - 2023-04_24 - Onwards/Python/Stock Market Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_715DC1F9088BCA31BF2C4CBF85ED2F6D7876A4C7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E182DDD0-C41D-455F-A707-0CA5DAD02F75}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_715DC1F9088BCA31BF2C4C3295AD02DF7976A4C7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEBD7DA7-8973-497B-A9A9-16467C37C247}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
developed unique ticket symbols df
</commit_message>
<xml_diff>
--- a/fundamentals_condensed_df.xlsx
+++ b/fundamentals_condensed_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25ac2033dcfcea55/Desktop/ALIENWARE - 2023-04_24 - Onwards/Python/Stock Market Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_715DC1F9088BCA31BF2C4C93EDEA392D7976A4C7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{222F3B8F-37C9-47B0-AE01-97B590BA6459}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_715DC1F9088BCA31BF2C4C671D6F0D0F7876A4C7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F1A8518-6137-45BA-810A-EA0B17A9554D}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
removed unique ticker symbols list df
</commit_message>
<xml_diff>
--- a/fundamentals_condensed_df.xlsx
+++ b/fundamentals_condensed_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25ac2033dcfcea55/Desktop/ALIENWARE - 2023-04_24 - Onwards/Python/Stock Market Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_715DC1F9088BCA31BF2C4C671D6F0D0F7876A4C7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F1A8518-6137-45BA-810A-EA0B17A9554D}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_715DC1F9088BCA31BF2C4C1FC52922AD7876A4C7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE8CD03F-FDFF-47B6-B0E5-36410D5E67C9}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
developed dataframes pertaining to positive yearly earnings
</commit_message>
<xml_diff>
--- a/fundamentals_condensed_df.xlsx
+++ b/fundamentals_condensed_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25ac2033dcfcea55/Desktop/ALIENWARE - 2023-04_24 - Onwards/Python/Stock Market Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_715DC1F9088BCA31BF2C4C207D2A334F7976A4C7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25E1CBAA-A864-49DE-9E60-53C51C94B525}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_715DC1F9088BCA31BF2C4C6E5D6E22BD7976A4C7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{169FD313-6451-4BD4-A0B3-16F85F70771A}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>